<commit_message>
enhance send data to arduino
</commit_message>
<xml_diff>
--- a/2024_11_06.xlsx
+++ b/2024_11_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1657,6 +1657,1518 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>111</v>
+      </c>
+      <c r="B59" t="n">
+        <v>222</v>
+      </c>
+      <c r="C59" t="n">
+        <v>2</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>64</v>
+      </c>
+      <c r="B60" t="n">
+        <v>157</v>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-34</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>105</v>
+      </c>
+      <c r="B61" t="n">
+        <v>215</v>
+      </c>
+      <c r="C61" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-35</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>154</v>
+      </c>
+      <c r="C62" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>67</v>
+      </c>
+      <c r="B63" t="n">
+        <v>154</v>
+      </c>
+      <c r="C63" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>93</v>
+      </c>
+      <c r="B64" t="n">
+        <v>207</v>
+      </c>
+      <c r="C64" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>136</v>
+      </c>
+      <c r="B65" t="n">
+        <v>201</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-50-41</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>81</v>
+      </c>
+      <c r="B66" t="n">
+        <v>166</v>
+      </c>
+      <c r="C66" t="n">
+        <v>3</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>87</v>
+      </c>
+      <c r="B67" t="n">
+        <v>184</v>
+      </c>
+      <c r="C67" t="n">
+        <v>3</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>113</v>
+      </c>
+      <c r="B68" t="n">
+        <v>212</v>
+      </c>
+      <c r="C68" t="n">
+        <v>3</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>73</v>
+      </c>
+      <c r="B69" t="n">
+        <v>146</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-35</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>76</v>
+      </c>
+      <c r="B70" t="n">
+        <v>159</v>
+      </c>
+      <c r="C70" t="n">
+        <v>2</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>167</v>
+      </c>
+      <c r="B71" t="n">
+        <v>211</v>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-51-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>82</v>
+      </c>
+      <c r="B72" t="n">
+        <v>192</v>
+      </c>
+      <c r="C72" t="n">
+        <v>3</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-52-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>82</v>
+      </c>
+      <c r="B73" t="n">
+        <v>192</v>
+      </c>
+      <c r="C73" t="n">
+        <v>3</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-52-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>107</v>
+      </c>
+      <c r="B74" t="n">
+        <v>225</v>
+      </c>
+      <c r="C74" t="n">
+        <v>3</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-52-52</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>59</v>
+      </c>
+      <c r="B75" t="n">
+        <v>116</v>
+      </c>
+      <c r="C75" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-53-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>90</v>
+      </c>
+      <c r="B76" t="n">
+        <v>187</v>
+      </c>
+      <c r="C76" t="n">
+        <v>2</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-53-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>82</v>
+      </c>
+      <c r="B77" t="n">
+        <v>186</v>
+      </c>
+      <c r="C77" t="n">
+        <v>2</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-54-53</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>111</v>
+      </c>
+      <c r="B78" t="n">
+        <v>219</v>
+      </c>
+      <c r="C78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>180</v>
+      </c>
+      <c r="B79" t="n">
+        <v>201</v>
+      </c>
+      <c r="C79" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>193</v>
+      </c>
+      <c r="B80" t="n">
+        <v>145</v>
+      </c>
+      <c r="C80" t="n">
+        <v>2</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>196</v>
+      </c>
+      <c r="B81" t="n">
+        <v>127</v>
+      </c>
+      <c r="C81" t="n">
+        <v>2</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>198</v>
+      </c>
+      <c r="B82" t="n">
+        <v>124</v>
+      </c>
+      <c r="C82" t="n">
+        <v>2</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>196</v>
+      </c>
+      <c r="B83" t="n">
+        <v>126</v>
+      </c>
+      <c r="C83" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>196</v>
+      </c>
+      <c r="B84" t="n">
+        <v>126</v>
+      </c>
+      <c r="C84" t="n">
+        <v>2</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>196</v>
+      </c>
+      <c r="B85" t="n">
+        <v>127</v>
+      </c>
+      <c r="C85" t="n">
+        <v>2</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>196</v>
+      </c>
+      <c r="B86" t="n">
+        <v>127</v>
+      </c>
+      <c r="C86" t="n">
+        <v>2</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>196</v>
+      </c>
+      <c r="B87" t="n">
+        <v>127</v>
+      </c>
+      <c r="C87" t="n">
+        <v>2</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>196</v>
+      </c>
+      <c r="B88" t="n">
+        <v>127</v>
+      </c>
+      <c r="C88" t="n">
+        <v>2</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>196</v>
+      </c>
+      <c r="B89" t="n">
+        <v>128</v>
+      </c>
+      <c r="C89" t="n">
+        <v>2</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>196</v>
+      </c>
+      <c r="B90" t="n">
+        <v>128</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2024-11-06-17-59-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>196</v>
+      </c>
+      <c r="B91" t="n">
+        <v>126</v>
+      </c>
+      <c r="C91" t="n">
+        <v>2</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-00-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>98</v>
+      </c>
+      <c r="B92" t="n">
+        <v>232</v>
+      </c>
+      <c r="C92" t="n">
+        <v>2</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-51-55</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>62</v>
+      </c>
+      <c r="B93" t="n">
+        <v>121</v>
+      </c>
+      <c r="C93" t="n">
+        <v>4</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-53-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>73</v>
+      </c>
+      <c r="B94" t="n">
+        <v>377</v>
+      </c>
+      <c r="C94" t="n">
+        <v>4</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-53-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>138</v>
+      </c>
+      <c r="B95" t="n">
+        <v>265</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-54-00</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>78</v>
+      </c>
+      <c r="B96" t="n">
+        <v>173</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-54-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>73</v>
+      </c>
+      <c r="B97" t="n">
+        <v>153</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2024-11-06-18-57-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>141</v>
+      </c>
+      <c r="B98" t="n">
+        <v>228</v>
+      </c>
+      <c r="C98" t="n">
+        <v>2</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>92</v>
+      </c>
+      <c r="B99" t="n">
+        <v>199</v>
+      </c>
+      <c r="C99" t="n">
+        <v>2</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>90</v>
+      </c>
+      <c r="B100" t="n">
+        <v>197</v>
+      </c>
+      <c r="C100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>83</v>
+      </c>
+      <c r="B101" t="n">
+        <v>183</v>
+      </c>
+      <c r="C101" t="n">
+        <v>2</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>83</v>
+      </c>
+      <c r="B102" t="n">
+        <v>180</v>
+      </c>
+      <c r="C102" t="n">
+        <v>2</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>75</v>
+      </c>
+      <c r="B103" t="n">
+        <v>173</v>
+      </c>
+      <c r="C103" t="n">
+        <v>2</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>81</v>
+      </c>
+      <c r="B104" t="n">
+        <v>171</v>
+      </c>
+      <c r="C104" t="n">
+        <v>2</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-47</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>83</v>
+      </c>
+      <c r="B105" t="n">
+        <v>170</v>
+      </c>
+      <c r="C105" t="n">
+        <v>2</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-16-47</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>84</v>
+      </c>
+      <c r="B106" t="n">
+        <v>211</v>
+      </c>
+      <c r="C106" t="n">
+        <v>2</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-17-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>109</v>
+      </c>
+      <c r="B107" t="n">
+        <v>249</v>
+      </c>
+      <c r="C107" t="n">
+        <v>2</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-17-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>77</v>
+      </c>
+      <c r="B108" t="n">
+        <v>217</v>
+      </c>
+      <c r="C108" t="n">
+        <v>3</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-19-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>80</v>
+      </c>
+      <c r="B109" t="n">
+        <v>171</v>
+      </c>
+      <c r="C109" t="n">
+        <v>2</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>223</v>
+      </c>
+      <c r="B110" t="n">
+        <v>351</v>
+      </c>
+      <c r="C110" t="n">
+        <v>2</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>70</v>
+      </c>
+      <c r="B111" t="n">
+        <v>169</v>
+      </c>
+      <c r="C111" t="n">
+        <v>4</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>71</v>
+      </c>
+      <c r="B112" t="n">
+        <v>172</v>
+      </c>
+      <c r="C112" t="n">
+        <v>4</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>95</v>
+      </c>
+      <c r="B113" t="n">
+        <v>211</v>
+      </c>
+      <c r="C113" t="n">
+        <v>4</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>120</v>
+      </c>
+      <c r="B114" t="n">
+        <v>254</v>
+      </c>
+      <c r="C114" t="n">
+        <v>4</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>150</v>
+      </c>
+      <c r="B115" t="n">
+        <v>282</v>
+      </c>
+      <c r="C115" t="n">
+        <v>4</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-20-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>77</v>
+      </c>
+      <c r="B116" t="n">
+        <v>176</v>
+      </c>
+      <c r="C116" t="n">
+        <v>3</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>87</v>
+      </c>
+      <c r="B117" t="n">
+        <v>199</v>
+      </c>
+      <c r="C117" t="n">
+        <v>3</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>114</v>
+      </c>
+      <c r="B118" t="n">
+        <v>233</v>
+      </c>
+      <c r="C118" t="n">
+        <v>3</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>146</v>
+      </c>
+      <c r="B119" t="n">
+        <v>252</v>
+      </c>
+      <c r="C119" t="n">
+        <v>3</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>65</v>
+      </c>
+      <c r="B120" t="n">
+        <v>133</v>
+      </c>
+      <c r="C120" t="n">
+        <v>2</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-53</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>65</v>
+      </c>
+      <c r="B121" t="n">
+        <v>133</v>
+      </c>
+      <c r="C121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-53</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>75</v>
+      </c>
+      <c r="B122" t="n">
+        <v>160</v>
+      </c>
+      <c r="C122" t="n">
+        <v>2</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-54</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>80</v>
+      </c>
+      <c r="B123" t="n">
+        <v>178</v>
+      </c>
+      <c r="C123" t="n">
+        <v>2</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-54</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>87</v>
+      </c>
+      <c r="B124" t="n">
+        <v>199</v>
+      </c>
+      <c r="C124" t="n">
+        <v>2</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-54</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>98</v>
+      </c>
+      <c r="B125" t="n">
+        <v>217</v>
+      </c>
+      <c r="C125" t="n">
+        <v>2</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-55</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>102</v>
+      </c>
+      <c r="B126" t="n">
+        <v>224</v>
+      </c>
+      <c r="C126" t="n">
+        <v>2</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-55</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>114</v>
+      </c>
+      <c r="B127" t="n">
+        <v>241</v>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-55</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>118</v>
+      </c>
+      <c r="B128" t="n">
+        <v>247</v>
+      </c>
+      <c r="C128" t="n">
+        <v>2</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-55</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>192</v>
+      </c>
+      <c r="B129" t="n">
+        <v>273</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-21-56</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>100</v>
+      </c>
+      <c r="B130" t="n">
+        <v>245</v>
+      </c>
+      <c r="C130" t="n">
+        <v>2</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>2024-11-06-19-22-53</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>